<commit_message>
Docs ov 2022 3 Added results for Sapphire Rapids 6448Y. OV bench results and system config description (#15418)
fixes the FP32 and FP16 swap of results.

* SPR-6448Y updated results

Updated all files with data for SPR 6448Y. New results in benchmark-data.csv, benchmark-performance-data.xls, benchmark-info-detailed.xls and platform-list_22.3.pdf
</commit_message>
<xml_diff>
--- a/docs/_static/benchmarks_files/OV-2022.3-Performance-Data.xlsx
+++ b/docs/_static/benchmarks_files/OV-2022.3-Performance-Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18BC82EA-1E8A-4F25-9B5C-5062A0C18B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{5D4B3D3F-55F8-4EE1-94AC-0669040E6A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{849FF1CB-EC80-4DE3-8A3D-F1BE25B6D7DD}"/>
   <bookViews>
-    <workbookView xWindow="-34410" yWindow="975" windowWidth="28800" windowHeight="15570" tabRatio="881" activeTab="2" xr2:uid="{B749C7B1-8D5C-4F8B-BC14-943DC6A423EB}"/>
+    <workbookView xWindow="-34815" yWindow="1080" windowWidth="25905" windowHeight="14925" tabRatio="881" firstSheet="2" activeTab="9" xr2:uid="{B749C7B1-8D5C-4F8B-BC14-943DC6A423EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="20" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="64">
   <si>
     <t>Results may vary. For workloads and configurations visit:</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Intel® Xeon® 6448Y</t>
+  </si>
+  <si>
+    <t>Test Date: January 14, 2023</t>
   </si>
 </sst>
 </file>
@@ -496,6 +502,7 @@
                   <c:v>Intel Atom®  X5-E3940 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -615,7 +622,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-8D06-4315-8461-AC6A3589DF62}"/>
             </c:ext>
@@ -633,6 +640,7 @@
                   <c:v>Intel® Atom®  X6425E INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -752,7 +760,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -770,6 +778,7 @@
                   <c:v>Intel® Celeron 6305E INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -889,7 +898,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -907,6 +916,7 @@
                   <c:v>Intel® Core™ i3-8100 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1026,7 +1036,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1044,6 +1054,7 @@
                   <c:v>Intel® Core™ i5-8500 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1163,7 +1174,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1181,6 +1192,7 @@
                   <c:v>Intel® Core™ i7-8700T INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1300,7 +1312,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1318,6 +1330,7 @@
                   <c:v>Intel® Core™ i9-10500TE INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1439,7 +1452,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1457,6 +1470,7 @@
                   <c:v>Intel® Core™ i9-10900TE INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1578,7 +1592,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1596,6 +1610,7 @@
                   <c:v>Intel® Core™ i7-1165G7 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1717,7 +1732,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1735,6 +1750,7 @@
                   <c:v>Intel® Core™ i9-12900K INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1856,7 +1872,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1874,6 +1890,7 @@
                   <c:v>Intel® Xeon® E-2124G INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1996,7 +2013,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2014,6 +2031,7 @@
                   <c:v>Intel® Xeon® W1290P INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2136,7 +2154,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2154,6 +2172,7 @@
                   <c:v>Intel® Xeon® Silver 4216R INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2276,7 +2295,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2294,6 +2313,7 @@
                   <c:v>Intel® Xeon® Gold 5218T INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2416,7 +2436,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2434,6 +2454,7 @@
                   <c:v>Intel® Xeon® Platinum 8270 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2556,7 +2577,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000010-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2703,8 +2724,147 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="9"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$K$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel® Xeon® 6448Y INT8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>bert-base-cased</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bert-large-uncased-whole-word-masking-squad-0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>deeplabv3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>densenet-121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>efficientdet-d0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>faster_rcnn_resnet50_coco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>inception-v4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mobilenet-ssd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mobilenet-v2-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>renset-18-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>resnet-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ssd-resnet34-1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unet-camvid-onnx-0001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>yolo_v3_tiny</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>yolo_v4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Tables  CPU'!$B$291:$B$305</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2090.7600000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>651.95000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1139.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8279.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>875.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>282.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3406.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16445.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28383.759999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27331.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11359.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>152.74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>381.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7344.88</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>252.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD3B-4CDC-9150-AD2E21BBC36A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="18"/>
-          <c:order val="16"/>
+          <c:order val="17"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$2</c:f>
@@ -2714,6 +2874,7 @@
                   <c:v>Intel Atom®  X5-E3940 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2835,7 +2996,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2843,7 +3004,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="19"/>
-          <c:order val="17"/>
+          <c:order val="18"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$18</c:f>
@@ -2853,6 +3014,7 @@
                   <c:v>Intel® Atom®  X6425E FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2974,7 +3136,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000013-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2982,7 +3144,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="20"/>
-          <c:order val="18"/>
+          <c:order val="19"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$34</c:f>
@@ -2992,6 +3154,7 @@
                   <c:v>Intel® Celeron 6305E FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3113,7 +3276,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000014-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3121,7 +3284,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="21"/>
-          <c:order val="19"/>
+          <c:order val="20"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$50</c:f>
@@ -3131,6 +3294,7 @@
                   <c:v>Intel® Core™ i3-8100 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3252,7 +3416,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000015-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3260,7 +3424,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="23"/>
-          <c:order val="20"/>
+          <c:order val="21"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$66</c:f>
@@ -3270,6 +3434,7 @@
                   <c:v>Intel® Core™ i5-8500 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3391,7 +3556,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000017-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3399,7 +3564,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="22"/>
-          <c:order val="21"/>
+          <c:order val="22"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$82</c:f>
@@ -3409,6 +3574,7 @@
                   <c:v>Intel® Core™ i7-8700T FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3530,7 +3696,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000016-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3538,7 +3704,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="24"/>
-          <c:order val="22"/>
+          <c:order val="23"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$98</c:f>
@@ -3548,6 +3714,7 @@
                   <c:v>Intel® Core™ i9-10500TE FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3670,7 +3837,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000018-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3678,7 +3845,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="25"/>
-          <c:order val="23"/>
+          <c:order val="24"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$114</c:f>
@@ -3688,6 +3855,7 @@
                   <c:v>Intel® Core™ i9-10900TE FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3810,7 +3978,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000019-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3818,7 +3986,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="26"/>
-          <c:order val="24"/>
+          <c:order val="25"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$130</c:f>
@@ -3828,6 +3996,7 @@
                   <c:v>Intel® Core™ i7-1165G7 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3950,7 +4119,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001A-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3958,7 +4127,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="28"/>
-          <c:order val="25"/>
+          <c:order val="26"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$162</c:f>
@@ -3968,6 +4137,7 @@
                   <c:v>Intel® Core™ i9-12900K FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4090,7 +4260,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001C-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4098,7 +4268,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="30"/>
-          <c:order val="26"/>
+          <c:order val="27"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$194</c:f>
@@ -4108,6 +4278,7 @@
                   <c:v>Intel® Xeon® E-2124G FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4229,7 +4400,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001E-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4237,7 +4408,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="31"/>
-          <c:order val="27"/>
+          <c:order val="28"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$210</c:f>
@@ -4247,6 +4418,7 @@
                   <c:v>Intel® Xeon® W1290P FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4368,7 +4540,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001F-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4376,7 +4548,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="32"/>
-          <c:order val="28"/>
+          <c:order val="29"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$226</c:f>
@@ -4386,6 +4558,7 @@
                   <c:v>Intel® Xeon® Silver 4216R FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4507,7 +4680,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000020-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4515,7 +4688,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="33"/>
-          <c:order val="29"/>
+          <c:order val="30"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$242</c:f>
@@ -4525,6 +4698,7 @@
                   <c:v>Intel® Xeon® Gold 5218T FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4646,7 +4820,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000021-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4654,7 +4828,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="34"/>
-          <c:order val="30"/>
+          <c:order val="31"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$258</c:f>
@@ -4664,6 +4838,7 @@
                   <c:v>Intel® Xeon® Platinum 8270 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4785,7 +4960,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000022-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4793,7 +4968,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="35"/>
-          <c:order val="31"/>
+          <c:order val="32"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$274</c:f>
@@ -4803,6 +4978,7 @@
                   <c:v>Intel® Xeon® 6336Y FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4924,9 +5100,149 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000023-93F2-4A08-B098-CCF5E12A5FF5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="33"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$L$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel® Xeon® 6448Y FP32</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>bert-base-cased</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bert-large-uncased-whole-word-masking-squad-0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>deeplabv3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>densenet-121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>efficientdet-d0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>faster_rcnn_resnet50_coco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>inception-v4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mobilenet-ssd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mobilenet-v2-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>renset-18-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>resnet-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ssd-resnet34-1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unet-camvid-onnx-0001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>yolo_v3_tiny</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>yolo_v4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Tables  CPU'!$C$291:$C$305</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>326.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>271.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1137.4100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>560.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2736.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7254.28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2329.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1118.97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1405.51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>58.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD3B-4CDC-9150-AD2E21BBC36A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10817,6 +11133,145 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000014-F1FF-46EE-AEA2-4BFCD47352F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$G$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel® Xeon® 6448Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>bert-base-cased</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bert-large-uncased-whole-word-masking-squad-0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>deeplabv3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>densenet-121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>efficientdet-d0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>faster_rcnn_resnet50_coco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>inception-v4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mobilenet-ssd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mobilenet-v2-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>renset-18-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>resnet-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ssd-resnet34-1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unet-camvid-onnx-0001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>yolo_v3_tiny</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>yolo_v4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Tables  CPU'!$D$291:$D$305</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.6100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1E0-4123-BE62-60911BFBD249}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -22135,13 +22590,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>430530</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>118110</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22729,12 +23184,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FdLYrnpYGMoZGEGiCaHR77z9+PjuW78HWMyldxC7t8MwsOYsQDcoHD31rnNUjj4GaNyDA6FgowKG3czkg0T2FA==" saltValue="oRU7cZT0PvcvSsvgGvQQtw==" spinCount="100000" sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -22743,11 +23198,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4557519A-0F83-4055-96A6-F175C564EF10}">
-  <dimension ref="A1:N289"/>
+  <dimension ref="A1:N305"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E296" sqref="E296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22768,7 +23223,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>8</v>
@@ -33855,8 +34310,612 @@
       <c r="K289" s="15"/>
       <c r="L289" s="15"/>
     </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G290" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H290" s="18">
+        <v>2</v>
+      </c>
+      <c r="I290" s="15"/>
+      <c r="J290" s="15"/>
+      <c r="K290" s="15" t="str">
+        <f>CONCATENATE(G290, ," ", B290)</f>
+        <v>Intel® Xeon® 6448Y INT8</v>
+      </c>
+      <c r="L290" s="15" t="str">
+        <f>CONCATENATE($G290, ," ", C290)</f>
+        <v>Intel® Xeon® 6448Y FP32</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="str">
+        <f>$A$3</f>
+        <v>bert-base-cased</v>
+      </c>
+      <c r="B291" s="12">
+        <v>2090.7600000000002</v>
+      </c>
+      <c r="C291" s="12">
+        <v>326.55</v>
+      </c>
+      <c r="D291" s="12">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E291" s="4">
+        <f t="shared" ref="E291:E305" si="160">B291/(I291*H291)</f>
+        <v>0.29176109405526096</v>
+      </c>
+      <c r="F291" s="4">
+        <f t="shared" ref="F291:F305" si="161">B291/(H291*J291)</f>
+        <v>4.6461333333333341</v>
+      </c>
+      <c r="G291" s="2"/>
+      <c r="H291" s="18">
+        <f t="shared" ref="H291:J305" si="162">H290</f>
+        <v>2</v>
+      </c>
+      <c r="I291" s="15">
+        <v>3583</v>
+      </c>
+      <c r="J291" s="15">
+        <v>225</v>
+      </c>
+      <c r="K291" s="15"/>
+      <c r="L291" s="15"/>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A292" s="3" t="str">
+        <f>$A$4</f>
+        <v>bert-large-uncased-whole-word-masking-squad-0001</v>
+      </c>
+      <c r="B292" s="12">
+        <v>651.95000000000005</v>
+      </c>
+      <c r="C292" s="12">
+        <v>91.18</v>
+      </c>
+      <c r="D292" s="12">
+        <v>12.87</v>
+      </c>
+      <c r="E292" s="4">
+        <f t="shared" si="160"/>
+        <v>9.0978230533072857E-2</v>
+      </c>
+      <c r="F292" s="4">
+        <f t="shared" si="161"/>
+        <v>1.4487777777777779</v>
+      </c>
+      <c r="G292" s="2"/>
+      <c r="H292" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I292" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J292" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K292" s="15"/>
+      <c r="L292" s="15"/>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="str">
+        <f>$A$5</f>
+        <v>deeplabv3</v>
+      </c>
+      <c r="B293" s="12">
+        <v>1139.5</v>
+      </c>
+      <c r="C293" s="12">
+        <v>271.62</v>
+      </c>
+      <c r="D293" s="12">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E293" s="4">
+        <f t="shared" si="160"/>
+        <v>0.15901479207368127</v>
+      </c>
+      <c r="F293" s="4">
+        <f t="shared" si="161"/>
+        <v>2.5322222222222224</v>
+      </c>
+      <c r="G293" s="3"/>
+      <c r="H293" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I293" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J293" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K293" s="15"/>
+      <c r="L293" s="15"/>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="str">
+        <f>$A$6</f>
+        <v>densenet-121</v>
+      </c>
+      <c r="B294" s="12">
+        <v>8279.14</v>
+      </c>
+      <c r="C294" s="12">
+        <v>1137.4100000000001</v>
+      </c>
+      <c r="D294" s="12">
+        <v>2.39</v>
+      </c>
+      <c r="E294" s="4">
+        <f t="shared" si="160"/>
+        <v>1.1553363103544514</v>
+      </c>
+      <c r="F294" s="4">
+        <f t="shared" si="161"/>
+        <v>18.398088888888889</v>
+      </c>
+      <c r="G294" s="3"/>
+      <c r="H294" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I294" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J294" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K294" s="15"/>
+      <c r="L294" s="15"/>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A295" s="3" t="str">
+        <f>$A$7</f>
+        <v>efficientdet-d0</v>
+      </c>
+      <c r="B295" s="12">
+        <v>875.53</v>
+      </c>
+      <c r="C295" s="12">
+        <v>560.48</v>
+      </c>
+      <c r="D295" s="12">
+        <v>5.05</v>
+      </c>
+      <c r="E295" s="4">
+        <f t="shared" si="160"/>
+        <v>0.12217834217136478</v>
+      </c>
+      <c r="F295" s="4">
+        <f t="shared" si="161"/>
+        <v>1.9456222222222221</v>
+      </c>
+      <c r="G295" s="3"/>
+      <c r="H295" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I295" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J295" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K295" s="15"/>
+      <c r="L295" s="15"/>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="str">
+        <f>$A$8</f>
+        <v>faster_rcnn_resnet50_coco</v>
+      </c>
+      <c r="B296" s="12">
+        <v>282.45</v>
+      </c>
+      <c r="C296" s="12">
+        <v>32.43</v>
+      </c>
+      <c r="D296" s="12">
+        <v>12.03</v>
+      </c>
+      <c r="E296" s="4">
+        <f t="shared" si="160"/>
+        <v>3.9415294445994974E-2</v>
+      </c>
+      <c r="F296" s="4">
+        <f t="shared" si="161"/>
+        <v>0.6276666666666666</v>
+      </c>
+      <c r="G296" s="3"/>
+      <c r="H296" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I296" s="16">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J296" s="16">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K296" s="16"/>
+      <c r="L296" s="16"/>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="str">
+        <f>$A$9</f>
+        <v>inception-v4</v>
+      </c>
+      <c r="B297" s="12">
+        <v>3406.7</v>
+      </c>
+      <c r="C297" s="12">
+        <v>331.56</v>
+      </c>
+      <c r="D297" s="12">
+        <v>3.23</v>
+      </c>
+      <c r="E297" s="4">
+        <f t="shared" si="160"/>
+        <v>0.4753977114150153</v>
+      </c>
+      <c r="F297" s="4">
+        <f t="shared" si="161"/>
+        <v>7.5704444444444441</v>
+      </c>
+      <c r="G297" s="3"/>
+      <c r="H297" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I297" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J297" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K297" s="15"/>
+      <c r="L297" s="15"/>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A298" s="3" t="str">
+        <f>$A$10</f>
+        <v>mobilenet-ssd</v>
+      </c>
+      <c r="B298" s="12">
+        <v>16445.75</v>
+      </c>
+      <c r="C298" s="12">
+        <v>2736.2</v>
+      </c>
+      <c r="D298" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="E298" s="4">
+        <f t="shared" si="160"/>
+        <v>2.2949692994697179</v>
+      </c>
+      <c r="F298" s="4">
+        <f t="shared" si="161"/>
+        <v>36.546111111111109</v>
+      </c>
+      <c r="G298" s="3"/>
+      <c r="H298" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I298" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J298" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K298" s="15"/>
+      <c r="L298" s="15"/>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="str">
+        <f>$A$11</f>
+        <v>mobilenet-v2-pytorch</v>
+      </c>
+      <c r="B299" s="12">
+        <v>28383.759999999998</v>
+      </c>
+      <c r="C299" s="12">
+        <v>7254.28</v>
+      </c>
+      <c r="D299" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E299" s="4">
+        <f t="shared" si="160"/>
+        <v>3.9608931063354729</v>
+      </c>
+      <c r="F299" s="4">
+        <f t="shared" si="161"/>
+        <v>63.075022222222216</v>
+      </c>
+      <c r="G299" s="3"/>
+      <c r="H299" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I299" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J299" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K299" s="15"/>
+      <c r="L299" s="15"/>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="str">
+        <f>$A$12</f>
+        <v>renset-18-pytorch</v>
+      </c>
+      <c r="B300" s="12">
+        <v>27331.02</v>
+      </c>
+      <c r="C300" s="12">
+        <v>2329.12</v>
+      </c>
+      <c r="D300" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="E300" s="4">
+        <f t="shared" si="160"/>
+        <v>3.8139854870220486</v>
+      </c>
+      <c r="F300" s="4">
+        <f t="shared" si="161"/>
+        <v>60.735599999999998</v>
+      </c>
+      <c r="G300" s="3"/>
+      <c r="H300" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I300" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J300" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K300" s="15"/>
+      <c r="L300" s="15"/>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="str">
+        <f>$A$13</f>
+        <v>resnet-50</v>
+      </c>
+      <c r="B301" s="12">
+        <v>11359.88</v>
+      </c>
+      <c r="C301" s="12">
+        <v>1118.97</v>
+      </c>
+      <c r="D301" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="E301" s="4">
+        <f t="shared" si="160"/>
+        <v>1.5852469997209042</v>
+      </c>
+      <c r="F301" s="4">
+        <f t="shared" si="161"/>
+        <v>25.244177777777775</v>
+      </c>
+      <c r="G301" s="3"/>
+      <c r="H301" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I301" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J301" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K301" s="15"/>
+      <c r="L301" s="15"/>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="str">
+        <f>$A$14</f>
+        <v>ssd-resnet34-1200</v>
+      </c>
+      <c r="B302" s="12">
+        <v>152.74</v>
+      </c>
+      <c r="C302" s="12">
+        <v>20.32</v>
+      </c>
+      <c r="D302" s="12">
+        <v>14.48</v>
+      </c>
+      <c r="E302" s="4">
+        <f t="shared" si="160"/>
+        <v>2.1314540887524422E-2</v>
+      </c>
+      <c r="F302" s="4">
+        <f t="shared" si="161"/>
+        <v>0.33942222222222224</v>
+      </c>
+      <c r="G302" s="3"/>
+      <c r="H302" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I302" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J302" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K302" s="15"/>
+      <c r="L302" s="15"/>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A303" s="3" t="str">
+        <f>$A$15</f>
+        <v>unet-camvid-onnx-0001</v>
+      </c>
+      <c r="B303" s="12">
+        <v>381.85</v>
+      </c>
+      <c r="C303" s="12">
+        <v>30.96</v>
+      </c>
+      <c r="D303" s="12">
+        <v>7.95</v>
+      </c>
+      <c r="E303" s="4">
+        <f t="shared" si="160"/>
+        <v>5.3286352218811055E-2</v>
+      </c>
+      <c r="F303" s="4">
+        <f t="shared" si="161"/>
+        <v>0.84855555555555562</v>
+      </c>
+      <c r="G303" s="3"/>
+      <c r="H303" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I303" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J303" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K303" s="15"/>
+      <c r="L303" s="15"/>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="str">
+        <f>$A$16</f>
+        <v>yolo_v3_tiny</v>
+      </c>
+      <c r="B304" s="12">
+        <v>7344.88</v>
+      </c>
+      <c r="C304" s="12">
+        <v>1405.51</v>
+      </c>
+      <c r="D304" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="E304" s="4">
+        <f t="shared" si="160"/>
+        <v>1.0249623220764723</v>
+      </c>
+      <c r="F304" s="4">
+        <f t="shared" si="161"/>
+        <v>16.321955555555554</v>
+      </c>
+      <c r="G304" s="3"/>
+      <c r="H304" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I304" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J304" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K304" s="15"/>
+      <c r="L304" s="15"/>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="str">
+        <f>$A$17</f>
+        <v>yolo_v4</v>
+      </c>
+      <c r="B305" s="12">
+        <v>252.03</v>
+      </c>
+      <c r="C305" s="12">
+        <v>58.12</v>
+      </c>
+      <c r="D305" s="12">
+        <v>15.01</v>
+      </c>
+      <c r="E305" s="4">
+        <f t="shared" si="160"/>
+        <v>3.5170248395199555E-2</v>
+      </c>
+      <c r="F305" s="4">
+        <f t="shared" si="161"/>
+        <v>0.56006666666666671</v>
+      </c>
+      <c r="G305" s="3"/>
+      <c r="H305" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I305" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J305" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K305" s="15"/>
+      <c r="L305" s="15"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zWKfsw3kv4IuQDxxhJ7HXiaM2aTBvZZr+7YA3KpRyN1prOPzSPyt4N2NLtVV4FLM6HAemn9i+A1QpSwaCzJCrQ==" saltValue="r3Kv+sNLNWmldW/5jc8yzg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SNIz7Lid+ZfWQ7Mvo+iKvvjhrgQ/zpbdcbUhYwhlPQ+qZqf2o1GdFhjWLHCmBDBb65qv5jRELDry8CpmWQdwAQ==" saltValue="hkGJMnbTpfwn5MoUSUmjzA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="H1" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="M1" name="Range1_1_1_1"/>
@@ -33879,8 +34938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F06CD1-752B-498F-9798-12B0324B9F85}">
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87:F102"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36979,7 +38038,7 @@
       <c r="G146" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GBGfXWo4PoQc+Ti3l2H4PaQyWCsWkzSm1izsZS2Cajl24FEve/Tlb5pT2oMPvbkCexp/mNkTSxFHfcHWWobr0g==" saltValue="HYvwjbJ7RvBNGNllu2ENAw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4Qzp26ayH71obZOvGbNXBqX0hvJtXBZvN2pJDxCMEjvw+U5BZKSTHuzoJFOrBd8S5ayLDfz+YJzJpgi+7eaHDQ==" saltValue="LpEbzAIEsPW4ZD8bTJAYrw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="K1" name="Range1_1_1"/>
   </protectedRanges>
@@ -38512,7 +39571,7 @@
       <c r="F113" s="20"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MR1w+TEoSVKAAd7u17yUbblkGHVMRJC+/ChIuPXc1sVlHukfjt4O+q7Hi3dO0BE7FZ7D0vzhTC48A33P6lAxPQ==" saltValue="GC8VfwO3w+mTBaqxGs4lFQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0MWztbKEjercUXDwfauokp/ItRZbirRdn1HmWqbOgBdK9Dc0alzbaS41fhElNA58VqBiG4ZXknyw0OU82vj/hg==" saltValue="omiJicerOkL4qVRRWqOT6g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="H1" name="Range1_1_1"/>
   </protectedRanges>
@@ -38542,7 +39601,7 @@
       <c r="B19" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xaZSwPIurNYlkNFACbsaICJco+L1sFjRg5VjUjrsKLd6YWg+zUUWZCbSobK3tAohU3zJNSQMF6iDg1fiLuV9AA==" saltValue="62sRoLVTDWSPdsc58Pjs8w==" spinCount="100000" sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -38553,7 +39612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D78DB2A-D305-45E8-BD60-3D75722BA7F9}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -38567,7 +39626,7 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -38759,7 +39818,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38774,7 +39833,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -38834,9 +39893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89A2D0C-443E-4F4D-930F-9417DFA35BE1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -38919,7 +39976,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -38988,7 +40045,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Docs ov 2022 3 Added results for Sapphire Rapids 6448Y. OV bench results and system config description (#15418) (#15443)
fixes the FP32 and FP16 swap of results.

* SPR-6448Y updated results

Updated all files with data for SPR 6448Y. New results in benchmark-data.csv, benchmark-performance-data.xls, benchmark-info-detailed.xls and platform-list_22.3.pdf

authored-by: Michael Frank Hansen <michael.f.hansen@intel.com>
</commit_message>
<xml_diff>
--- a/docs/_static/benchmarks_files/OV-2022.3-Performance-Data.xlsx
+++ b/docs/_static/benchmarks_files/OV-2022.3-Performance-Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18BC82EA-1E8A-4F25-9B5C-5062A0C18B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{5D4B3D3F-55F8-4EE1-94AC-0669040E6A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{849FF1CB-EC80-4DE3-8A3D-F1BE25B6D7DD}"/>
   <bookViews>
-    <workbookView xWindow="-34410" yWindow="975" windowWidth="28800" windowHeight="15570" tabRatio="881" activeTab="2" xr2:uid="{B749C7B1-8D5C-4F8B-BC14-943DC6A423EB}"/>
+    <workbookView xWindow="-34815" yWindow="1080" windowWidth="25905" windowHeight="14925" tabRatio="881" firstSheet="2" activeTab="9" xr2:uid="{B749C7B1-8D5C-4F8B-BC14-943DC6A423EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="20" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="64">
   <si>
     <t>Results may vary. For workloads and configurations visit:</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Intel® Xeon® 6448Y</t>
+  </si>
+  <si>
+    <t>Test Date: January 14, 2023</t>
   </si>
 </sst>
 </file>
@@ -496,6 +502,7 @@
                   <c:v>Intel Atom®  X5-E3940 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -615,7 +622,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-8D06-4315-8461-AC6A3589DF62}"/>
             </c:ext>
@@ -633,6 +640,7 @@
                   <c:v>Intel® Atom®  X6425E INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -752,7 +760,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -770,6 +778,7 @@
                   <c:v>Intel® Celeron 6305E INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -889,7 +898,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -907,6 +916,7 @@
                   <c:v>Intel® Core™ i3-8100 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1026,7 +1036,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1044,6 +1054,7 @@
                   <c:v>Intel® Core™ i5-8500 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1163,7 +1174,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1181,6 +1192,7 @@
                   <c:v>Intel® Core™ i7-8700T INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1300,7 +1312,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1318,6 +1330,7 @@
                   <c:v>Intel® Core™ i9-10500TE INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1439,7 +1452,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1457,6 +1470,7 @@
                   <c:v>Intel® Core™ i9-10900TE INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1578,7 +1592,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1596,6 +1610,7 @@
                   <c:v>Intel® Core™ i7-1165G7 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1717,7 +1732,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1735,6 +1750,7 @@
                   <c:v>Intel® Core™ i9-12900K INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1856,7 +1872,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000A-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -1874,6 +1890,7 @@
                   <c:v>Intel® Xeon® E-2124G INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -1996,7 +2013,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000C-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2014,6 +2031,7 @@
                   <c:v>Intel® Xeon® W1290P INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2136,7 +2154,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2154,6 +2172,7 @@
                   <c:v>Intel® Xeon® Silver 4216R INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2276,7 +2295,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000E-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2294,6 +2313,7 @@
                   <c:v>Intel® Xeon® Gold 5218T INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2416,7 +2436,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000F-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2434,6 +2454,7 @@
                   <c:v>Intel® Xeon® Platinum 8270 INT8</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2556,7 +2577,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000010-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2703,8 +2724,147 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="9"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$K$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel® Xeon® 6448Y INT8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>bert-base-cased</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bert-large-uncased-whole-word-masking-squad-0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>deeplabv3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>densenet-121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>efficientdet-d0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>faster_rcnn_resnet50_coco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>inception-v4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mobilenet-ssd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mobilenet-v2-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>renset-18-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>resnet-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ssd-resnet34-1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unet-camvid-onnx-0001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>yolo_v3_tiny</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>yolo_v4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Tables  CPU'!$B$291:$B$305</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2090.7600000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>651.95000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1139.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8279.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>875.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>282.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3406.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16445.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28383.759999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27331.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11359.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>152.74</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>381.85</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7344.88</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>252.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FD3B-4CDC-9150-AD2E21BBC36A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="18"/>
-          <c:order val="16"/>
+          <c:order val="17"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$2</c:f>
@@ -2714,6 +2874,7 @@
                   <c:v>Intel Atom®  X5-E3940 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2835,7 +2996,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000012-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2843,7 +3004,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="19"/>
-          <c:order val="17"/>
+          <c:order val="18"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$18</c:f>
@@ -2853,6 +3014,7 @@
                   <c:v>Intel® Atom®  X6425E FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2974,7 +3136,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000013-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -2982,7 +3144,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="20"/>
-          <c:order val="18"/>
+          <c:order val="19"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$34</c:f>
@@ -2992,6 +3154,7 @@
                   <c:v>Intel® Celeron 6305E FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3113,7 +3276,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000014-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3121,7 +3284,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="21"/>
-          <c:order val="19"/>
+          <c:order val="20"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$50</c:f>
@@ -3131,6 +3294,7 @@
                   <c:v>Intel® Core™ i3-8100 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3252,7 +3416,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000015-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3260,7 +3424,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="23"/>
-          <c:order val="20"/>
+          <c:order val="21"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$66</c:f>
@@ -3270,6 +3434,7 @@
                   <c:v>Intel® Core™ i5-8500 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3391,7 +3556,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000017-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3399,7 +3564,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="22"/>
-          <c:order val="21"/>
+          <c:order val="22"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$82</c:f>
@@ -3409,6 +3574,7 @@
                   <c:v>Intel® Core™ i7-8700T FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3530,7 +3696,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000016-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3538,7 +3704,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="24"/>
-          <c:order val="22"/>
+          <c:order val="23"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$98</c:f>
@@ -3548,6 +3714,7 @@
                   <c:v>Intel® Core™ i9-10500TE FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3670,7 +3837,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000018-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3678,7 +3845,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="25"/>
-          <c:order val="23"/>
+          <c:order val="24"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$114</c:f>
@@ -3688,6 +3855,7 @@
                   <c:v>Intel® Core™ i9-10900TE FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3810,7 +3978,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000019-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3818,7 +3986,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="26"/>
-          <c:order val="24"/>
+          <c:order val="25"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$130</c:f>
@@ -3828,6 +3996,7 @@
                   <c:v>Intel® Core™ i7-1165G7 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -3950,7 +4119,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001A-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -3958,7 +4127,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="28"/>
-          <c:order val="25"/>
+          <c:order val="26"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$162</c:f>
@@ -3968,6 +4137,7 @@
                   <c:v>Intel® Core™ i9-12900K FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4090,7 +4260,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001C-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4098,7 +4268,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="30"/>
-          <c:order val="26"/>
+          <c:order val="27"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$194</c:f>
@@ -4108,6 +4278,7 @@
                   <c:v>Intel® Xeon® E-2124G FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4229,7 +4400,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001E-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4237,7 +4408,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="31"/>
-          <c:order val="27"/>
+          <c:order val="28"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$210</c:f>
@@ -4247,6 +4418,7 @@
                   <c:v>Intel® Xeon® W1290P FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4368,7 +4540,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001F-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4376,7 +4548,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="32"/>
-          <c:order val="28"/>
+          <c:order val="29"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$226</c:f>
@@ -4386,6 +4558,7 @@
                   <c:v>Intel® Xeon® Silver 4216R FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4507,7 +4680,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000020-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4515,7 +4688,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="33"/>
-          <c:order val="29"/>
+          <c:order val="30"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$242</c:f>
@@ -4525,6 +4698,7 @@
                   <c:v>Intel® Xeon® Gold 5218T FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4646,7 +4820,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000021-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4654,7 +4828,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="34"/>
-          <c:order val="30"/>
+          <c:order val="31"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$258</c:f>
@@ -4664,6 +4838,7 @@
                   <c:v>Intel® Xeon® Platinum 8270 FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4785,7 +4960,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000022-93F2-4A08-B098-CCF5E12A5FF5}"/>
             </c:ext>
@@ -4793,7 +4968,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="35"/>
-          <c:order val="31"/>
+          <c:order val="32"/>
           <c:tx>
             <c:strRef>
               <c:f>'Performance Tables  CPU'!$L$274</c:f>
@@ -4803,6 +4978,7 @@
                   <c:v>Intel® Xeon® 6336Y FP32</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -4924,9 +5100,149 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000023-93F2-4A08-B098-CCF5E12A5FF5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="33"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$L$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel® Xeon® 6448Y FP32</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>bert-base-cased</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bert-large-uncased-whole-word-masking-squad-0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>deeplabv3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>densenet-121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>efficientdet-d0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>faster_rcnn_resnet50_coco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>inception-v4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mobilenet-ssd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mobilenet-v2-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>renset-18-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>resnet-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ssd-resnet34-1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unet-camvid-onnx-0001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>yolo_v3_tiny</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>yolo_v4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Tables  CPU'!$C$291:$C$305</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>326.55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>271.62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1137.4100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>560.48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>331.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2736.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7254.28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2329.12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1118.97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20.32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30.96</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1405.51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>58.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD3B-4CDC-9150-AD2E21BBC36A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10817,6 +11133,145 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000014-F1FF-46EE-AEA2-4BFCD47352F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$G$290</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Intel® Xeon® 6448Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Performance Tables  CPU'!$A$3:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>bert-base-cased</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>bert-large-uncased-whole-word-masking-squad-0001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>deeplabv3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>densenet-121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>efficientdet-d0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>faster_rcnn_resnet50_coco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>inception-v4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>mobilenet-ssd</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>mobilenet-v2-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>renset-18-pytorch</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>resnet-50</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ssd-resnet34-1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>unet-camvid-onnx-0001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>yolo_v3_tiny</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>yolo_v4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Performance Tables  CPU'!$D$291:$D$305</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.6100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.03</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1E0-4123-BE62-60911BFBD249}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -22135,13 +22590,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>430530</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>118110</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -22729,12 +23184,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FdLYrnpYGMoZGEGiCaHR77z9+PjuW78HWMyldxC7t8MwsOYsQDcoHD31rnNUjj4GaNyDA6FgowKG3czkg0T2FA==" saltValue="oRU7cZT0PvcvSsvgGvQQtw==" spinCount="100000" sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -22743,11 +23198,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4557519A-0F83-4055-96A6-F175C564EF10}">
-  <dimension ref="A1:N289"/>
+  <dimension ref="A1:N305"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E296" sqref="E296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22768,7 +23223,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>8</v>
@@ -33855,8 +34310,612 @@
       <c r="K289" s="15"/>
       <c r="L289" s="15"/>
     </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F290" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G290" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H290" s="18">
+        <v>2</v>
+      </c>
+      <c r="I290" s="15"/>
+      <c r="J290" s="15"/>
+      <c r="K290" s="15" t="str">
+        <f>CONCATENATE(G290, ," ", B290)</f>
+        <v>Intel® Xeon® 6448Y INT8</v>
+      </c>
+      <c r="L290" s="15" t="str">
+        <f>CONCATENATE($G290, ," ", C290)</f>
+        <v>Intel® Xeon® 6448Y FP32</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="str">
+        <f>$A$3</f>
+        <v>bert-base-cased</v>
+      </c>
+      <c r="B291" s="12">
+        <v>2090.7600000000002</v>
+      </c>
+      <c r="C291" s="12">
+        <v>326.55</v>
+      </c>
+      <c r="D291" s="12">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="E291" s="4">
+        <f t="shared" ref="E291:E305" si="160">B291/(I291*H291)</f>
+        <v>0.29176109405526096</v>
+      </c>
+      <c r="F291" s="4">
+        <f t="shared" ref="F291:F305" si="161">B291/(H291*J291)</f>
+        <v>4.6461333333333341</v>
+      </c>
+      <c r="G291" s="2"/>
+      <c r="H291" s="18">
+        <f t="shared" ref="H291:J305" si="162">H290</f>
+        <v>2</v>
+      </c>
+      <c r="I291" s="15">
+        <v>3583</v>
+      </c>
+      <c r="J291" s="15">
+        <v>225</v>
+      </c>
+      <c r="K291" s="15"/>
+      <c r="L291" s="15"/>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A292" s="3" t="str">
+        <f>$A$4</f>
+        <v>bert-large-uncased-whole-word-masking-squad-0001</v>
+      </c>
+      <c r="B292" s="12">
+        <v>651.95000000000005</v>
+      </c>
+      <c r="C292" s="12">
+        <v>91.18</v>
+      </c>
+      <c r="D292" s="12">
+        <v>12.87</v>
+      </c>
+      <c r="E292" s="4">
+        <f t="shared" si="160"/>
+        <v>9.0978230533072857E-2</v>
+      </c>
+      <c r="F292" s="4">
+        <f t="shared" si="161"/>
+        <v>1.4487777777777779</v>
+      </c>
+      <c r="G292" s="2"/>
+      <c r="H292" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I292" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J292" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K292" s="15"/>
+      <c r="L292" s="15"/>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="str">
+        <f>$A$5</f>
+        <v>deeplabv3</v>
+      </c>
+      <c r="B293" s="12">
+        <v>1139.5</v>
+      </c>
+      <c r="C293" s="12">
+        <v>271.62</v>
+      </c>
+      <c r="D293" s="12">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E293" s="4">
+        <f t="shared" si="160"/>
+        <v>0.15901479207368127</v>
+      </c>
+      <c r="F293" s="4">
+        <f t="shared" si="161"/>
+        <v>2.5322222222222224</v>
+      </c>
+      <c r="G293" s="3"/>
+      <c r="H293" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I293" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J293" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K293" s="15"/>
+      <c r="L293" s="15"/>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="str">
+        <f>$A$6</f>
+        <v>densenet-121</v>
+      </c>
+      <c r="B294" s="12">
+        <v>8279.14</v>
+      </c>
+      <c r="C294" s="12">
+        <v>1137.4100000000001</v>
+      </c>
+      <c r="D294" s="12">
+        <v>2.39</v>
+      </c>
+      <c r="E294" s="4">
+        <f t="shared" si="160"/>
+        <v>1.1553363103544514</v>
+      </c>
+      <c r="F294" s="4">
+        <f t="shared" si="161"/>
+        <v>18.398088888888889</v>
+      </c>
+      <c r="G294" s="3"/>
+      <c r="H294" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I294" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J294" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K294" s="15"/>
+      <c r="L294" s="15"/>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A295" s="3" t="str">
+        <f>$A$7</f>
+        <v>efficientdet-d0</v>
+      </c>
+      <c r="B295" s="12">
+        <v>875.53</v>
+      </c>
+      <c r="C295" s="12">
+        <v>560.48</v>
+      </c>
+      <c r="D295" s="12">
+        <v>5.05</v>
+      </c>
+      <c r="E295" s="4">
+        <f t="shared" si="160"/>
+        <v>0.12217834217136478</v>
+      </c>
+      <c r="F295" s="4">
+        <f t="shared" si="161"/>
+        <v>1.9456222222222221</v>
+      </c>
+      <c r="G295" s="3"/>
+      <c r="H295" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I295" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J295" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K295" s="15"/>
+      <c r="L295" s="15"/>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="str">
+        <f>$A$8</f>
+        <v>faster_rcnn_resnet50_coco</v>
+      </c>
+      <c r="B296" s="12">
+        <v>282.45</v>
+      </c>
+      <c r="C296" s="12">
+        <v>32.43</v>
+      </c>
+      <c r="D296" s="12">
+        <v>12.03</v>
+      </c>
+      <c r="E296" s="4">
+        <f t="shared" si="160"/>
+        <v>3.9415294445994974E-2</v>
+      </c>
+      <c r="F296" s="4">
+        <f t="shared" si="161"/>
+        <v>0.6276666666666666</v>
+      </c>
+      <c r="G296" s="3"/>
+      <c r="H296" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I296" s="16">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J296" s="16">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K296" s="16"/>
+      <c r="L296" s="16"/>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="str">
+        <f>$A$9</f>
+        <v>inception-v4</v>
+      </c>
+      <c r="B297" s="12">
+        <v>3406.7</v>
+      </c>
+      <c r="C297" s="12">
+        <v>331.56</v>
+      </c>
+      <c r="D297" s="12">
+        <v>3.23</v>
+      </c>
+      <c r="E297" s="4">
+        <f t="shared" si="160"/>
+        <v>0.4753977114150153</v>
+      </c>
+      <c r="F297" s="4">
+        <f t="shared" si="161"/>
+        <v>7.5704444444444441</v>
+      </c>
+      <c r="G297" s="3"/>
+      <c r="H297" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I297" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J297" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K297" s="15"/>
+      <c r="L297" s="15"/>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A298" s="3" t="str">
+        <f>$A$10</f>
+        <v>mobilenet-ssd</v>
+      </c>
+      <c r="B298" s="12">
+        <v>16445.75</v>
+      </c>
+      <c r="C298" s="12">
+        <v>2736.2</v>
+      </c>
+      <c r="D298" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="E298" s="4">
+        <f t="shared" si="160"/>
+        <v>2.2949692994697179</v>
+      </c>
+      <c r="F298" s="4">
+        <f t="shared" si="161"/>
+        <v>36.546111111111109</v>
+      </c>
+      <c r="G298" s="3"/>
+      <c r="H298" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I298" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J298" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K298" s="15"/>
+      <c r="L298" s="15"/>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="str">
+        <f>$A$11</f>
+        <v>mobilenet-v2-pytorch</v>
+      </c>
+      <c r="B299" s="12">
+        <v>28383.759999999998</v>
+      </c>
+      <c r="C299" s="12">
+        <v>7254.28</v>
+      </c>
+      <c r="D299" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E299" s="4">
+        <f t="shared" si="160"/>
+        <v>3.9608931063354729</v>
+      </c>
+      <c r="F299" s="4">
+        <f t="shared" si="161"/>
+        <v>63.075022222222216</v>
+      </c>
+      <c r="G299" s="3"/>
+      <c r="H299" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I299" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J299" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K299" s="15"/>
+      <c r="L299" s="15"/>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="str">
+        <f>$A$12</f>
+        <v>renset-18-pytorch</v>
+      </c>
+      <c r="B300" s="12">
+        <v>27331.02</v>
+      </c>
+      <c r="C300" s="12">
+        <v>2329.12</v>
+      </c>
+      <c r="D300" s="12">
+        <v>0.38</v>
+      </c>
+      <c r="E300" s="4">
+        <f t="shared" si="160"/>
+        <v>3.8139854870220486</v>
+      </c>
+      <c r="F300" s="4">
+        <f t="shared" si="161"/>
+        <v>60.735599999999998</v>
+      </c>
+      <c r="G300" s="3"/>
+      <c r="H300" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I300" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J300" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K300" s="15"/>
+      <c r="L300" s="15"/>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="str">
+        <f>$A$13</f>
+        <v>resnet-50</v>
+      </c>
+      <c r="B301" s="12">
+        <v>11359.88</v>
+      </c>
+      <c r="C301" s="12">
+        <v>1118.97</v>
+      </c>
+      <c r="D301" s="12">
+        <v>0.94</v>
+      </c>
+      <c r="E301" s="4">
+        <f t="shared" si="160"/>
+        <v>1.5852469997209042</v>
+      </c>
+      <c r="F301" s="4">
+        <f t="shared" si="161"/>
+        <v>25.244177777777775</v>
+      </c>
+      <c r="G301" s="3"/>
+      <c r="H301" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I301" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J301" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K301" s="15"/>
+      <c r="L301" s="15"/>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="str">
+        <f>$A$14</f>
+        <v>ssd-resnet34-1200</v>
+      </c>
+      <c r="B302" s="12">
+        <v>152.74</v>
+      </c>
+      <c r="C302" s="12">
+        <v>20.32</v>
+      </c>
+      <c r="D302" s="12">
+        <v>14.48</v>
+      </c>
+      <c r="E302" s="4">
+        <f t="shared" si="160"/>
+        <v>2.1314540887524422E-2</v>
+      </c>
+      <c r="F302" s="4">
+        <f t="shared" si="161"/>
+        <v>0.33942222222222224</v>
+      </c>
+      <c r="G302" s="3"/>
+      <c r="H302" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I302" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J302" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K302" s="15"/>
+      <c r="L302" s="15"/>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A303" s="3" t="str">
+        <f>$A$15</f>
+        <v>unet-camvid-onnx-0001</v>
+      </c>
+      <c r="B303" s="12">
+        <v>381.85</v>
+      </c>
+      <c r="C303" s="12">
+        <v>30.96</v>
+      </c>
+      <c r="D303" s="12">
+        <v>7.95</v>
+      </c>
+      <c r="E303" s="4">
+        <f t="shared" si="160"/>
+        <v>5.3286352218811055E-2</v>
+      </c>
+      <c r="F303" s="4">
+        <f t="shared" si="161"/>
+        <v>0.84855555555555562</v>
+      </c>
+      <c r="G303" s="3"/>
+      <c r="H303" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I303" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J303" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K303" s="15"/>
+      <c r="L303" s="15"/>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="str">
+        <f>$A$16</f>
+        <v>yolo_v3_tiny</v>
+      </c>
+      <c r="B304" s="12">
+        <v>7344.88</v>
+      </c>
+      <c r="C304" s="12">
+        <v>1405.51</v>
+      </c>
+      <c r="D304" s="12">
+        <v>1.06</v>
+      </c>
+      <c r="E304" s="4">
+        <f t="shared" si="160"/>
+        <v>1.0249623220764723</v>
+      </c>
+      <c r="F304" s="4">
+        <f t="shared" si="161"/>
+        <v>16.321955555555554</v>
+      </c>
+      <c r="G304" s="3"/>
+      <c r="H304" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I304" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J304" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K304" s="15"/>
+      <c r="L304" s="15"/>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="str">
+        <f>$A$17</f>
+        <v>yolo_v4</v>
+      </c>
+      <c r="B305" s="12">
+        <v>252.03</v>
+      </c>
+      <c r="C305" s="12">
+        <v>58.12</v>
+      </c>
+      <c r="D305" s="12">
+        <v>15.01</v>
+      </c>
+      <c r="E305" s="4">
+        <f t="shared" si="160"/>
+        <v>3.5170248395199555E-2</v>
+      </c>
+      <c r="F305" s="4">
+        <f t="shared" si="161"/>
+        <v>0.56006666666666671</v>
+      </c>
+      <c r="G305" s="3"/>
+      <c r="H305" s="18">
+        <f t="shared" si="162"/>
+        <v>2</v>
+      </c>
+      <c r="I305" s="15">
+        <f t="shared" si="162"/>
+        <v>3583</v>
+      </c>
+      <c r="J305" s="15">
+        <f t="shared" si="162"/>
+        <v>225</v>
+      </c>
+      <c r="K305" s="15"/>
+      <c r="L305" s="15"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zWKfsw3kv4IuQDxxhJ7HXiaM2aTBvZZr+7YA3KpRyN1prOPzSPyt4N2NLtVV4FLM6HAemn9i+A1QpSwaCzJCrQ==" saltValue="r3Kv+sNLNWmldW/5jc8yzg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SNIz7Lid+ZfWQ7Mvo+iKvvjhrgQ/zpbdcbUhYwhlPQ+qZqf2o1GdFhjWLHCmBDBb65qv5jRELDry8CpmWQdwAQ==" saltValue="hkGJMnbTpfwn5MoUSUmjzA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="H1" name="Range1"/>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="M1" name="Range1_1_1_1"/>
@@ -33879,8 +34938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F06CD1-752B-498F-9798-12B0324B9F85}">
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87:F102"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36979,7 +38038,7 @@
       <c r="G146" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GBGfXWo4PoQc+Ti3l2H4PaQyWCsWkzSm1izsZS2Cajl24FEve/Tlb5pT2oMPvbkCexp/mNkTSxFHfcHWWobr0g==" saltValue="HYvwjbJ7RvBNGNllu2ENAw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4Qzp26ayH71obZOvGbNXBqX0hvJtXBZvN2pJDxCMEjvw+U5BZKSTHuzoJFOrBd8S5ayLDfz+YJzJpgi+7eaHDQ==" saltValue="LpEbzAIEsPW4ZD8bTJAYrw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="K1" name="Range1_1_1"/>
   </protectedRanges>
@@ -38512,7 +39571,7 @@
       <c r="F113" s="20"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MR1w+TEoSVKAAd7u17yUbblkGHVMRJC+/ChIuPXc1sVlHukfjt4O+q7Hi3dO0BE7FZ7D0vzhTC48A33P6lAxPQ==" saltValue="GC8VfwO3w+mTBaqxGs4lFQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0MWztbKEjercUXDwfauokp/ItRZbirRdn1HmWqbOgBdK9Dc0alzbaS41fhElNA58VqBiG4ZXknyw0OU82vj/hg==" saltValue="omiJicerOkL4qVRRWqOT6g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="obtUc9z1SKpT2QgXGuBnBLMmP2Ruyrh4vLLC3J0+e2BoEQOdS3LNnQ1C54Wqf3ghA5JEEmSNQX0NVuijjCKrgA==" saltValue="t0gF7AecxnRApM1ODdLL/w==" spinCount="100000" sqref="H1" name="Range1_1_1"/>
   </protectedRanges>
@@ -38542,7 +39601,7 @@
       <c r="B19" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xaZSwPIurNYlkNFACbsaICJco+L1sFjRg5VjUjrsKLd6YWg+zUUWZCbSobK3tAohU3zJNSQMF6iDg1fiLuV9AA==" saltValue="62sRoLVTDWSPdsc58Pjs8w==" spinCount="100000" sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -38553,7 +39612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D78DB2A-D305-45E8-BD60-3D75722BA7F9}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -38567,7 +39626,7 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -38759,7 +39818,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38774,7 +39833,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -38834,9 +39893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89A2D0C-443E-4F4D-930F-9417DFA35BE1}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -38919,7 +39976,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -38988,7 +40045,7 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>'Performance Tables  CPU'!A1</f>
-        <v>Test Date: December 13, 2022</v>
+        <v>Test Date: January 14, 2023</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>

</xml_diff>